<commit_message>
Skill, Synergy 엑셀 파일 변경
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Skill/SkillDB/SkillBalanceTable.xlsx
+++ b/Assets/Scripts/Skill/SkillDB/SkillBalanceTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eunsu Park\UnityProject\Dragon_and_Test\Assets\Scripts\Player\Skill\SkillDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityProject\Dragon_and_Test\Assets\Scripts\Skill\SkillDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1A449F-BC20-4006-9DDF-4E5D48EFACE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9747FA34-3E60-4F8D-8965-FF9C28429BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{AEBFF8F3-8B34-44B4-8BD4-C39FC3DC70E4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{AEBFF8F3-8B34-44B4-8BD4-C39FC3DC70E4}"/>
   </bookViews>
   <sheets>
     <sheet name="SkillTableEntity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>cardName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,9 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>원형으로 넓게 펼쳐서 적을 넉백시키고 데미지를 준다</t>
-  </si>
-  <si>
     <t>JanCrane</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -125,6 +122,90 @@
   </si>
   <si>
     <t>force</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소나무잎을 올가미처럼 펼쳐 범위 내 적에게 슬로우와 데미지를 준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매화잎을 에이밍한 방향으로 발사해 적을 관통하며 데미지를 준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>벚꽃잎을 에이밍한 방향으로 발사해 적을 관통하며 데미지를 준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등나무 덩굴을 4방향으로 날려 몬스터를 관통하며 속박하고 데미지를 준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>난초잎을 올가미처럼 펼쳐 범위 내 적에게 슬로우와 데미지를 준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">모란잎을 원형으로 넓게 펼쳐서 적을 넉백시키고 데미지를 준다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>싸리잎을 2방향으로 에이밍한 쪽으로 발사해 적을 관통하며 데미지를 준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>억새 덩굴을 8방향으로 날려 몬스터를 관통하며 속박하고 데미지를 준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국화잎을 원형으로 넓게 펼쳐서 적을 넉백시키고 데미지를 준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단풍잎을 3방향으로 에이밍한 쪽으로 발사해 적을 관통하며 데미지를 준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소나무잎을 날리며 빠른 속도로 에이밍한 방향으로 이동한다. 이동중 무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매화잎을 날리며 빠른 속도로 에이밍한 방향으로 이동한다. 이동중 무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>벚꽃잎을 날리며 빠른 속도로 에이밍한 방향으로 이동한다. 이동중 무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등나무잎을 날리며 빠른 속도로 에이밍한 방향으로 이동한다. 이동중 무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>난초잎을 날리며 빠른 속도로 에이밍한 방향으로 이동한다. 이동중 무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모란잎을 날리며 빠른 속도로 에이밍한 방향으로 이동한다. 이동중 무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>싸리잎을 날리며 빠른 속도로 에이밍한 방향으로 이동한다. 이동중 무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>억새잎을 날리며 빠른 속도로 에이밍한 방향으로 이동한다. 이동중 무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국화잎을 날리며 빠른 속도로 에이밍한 방향으로 이동한다. 이동중 무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단풍잎을 날리며 빠른 속도로 에이밍한 방향으로 이동한다. 이동중 무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>duration</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -163,7 +244,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -186,13 +267,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -200,6 +305,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,19 +647,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17AA56DA-8172-46E9-A78E-2FEE4377866A}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="50.875" customWidth="1"/>
+    <col min="2" max="2" width="70.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -565,408 +676,405 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1">
-        <v>5</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
       </c>
-      <c r="D8" s="1">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="3">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E10" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F10" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1">
         <v>5</v>
       </c>
       <c r="D11" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1">
-        <v>10</v>
-      </c>
-      <c r="E13" s="1">
-        <v>5</v>
-      </c>
-      <c r="F13" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1">
+        <v>20</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1">
+        <v>20</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1">
-        <v>10</v>
-      </c>
-      <c r="E14" s="1">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1">
-        <v>3</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E15" s="1">
         <v>5</v>
       </c>
       <c r="F15" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1">
+        <v>20</v>
+      </c>
+      <c r="E16" s="1">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1">
+        <v>20</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1">
+        <v>20</v>
+      </c>
+      <c r="E18" s="1">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1">
+        <v>20</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1">
+        <v>20</v>
+      </c>
+      <c r="E19" s="1">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1">
         <v>10</v>
       </c>
-      <c r="E16" s="1">
-        <v>5</v>
-      </c>
-      <c r="F16" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1">
-        <v>10</v>
-      </c>
-      <c r="E17" s="1">
-        <v>5</v>
-      </c>
-      <c r="F17" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1">
-        <v>10</v>
-      </c>
-      <c r="E18" s="1">
-        <v>5</v>
-      </c>
-      <c r="F18" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1">
-        <v>3</v>
-      </c>
-      <c r="D19" s="1">
-        <v>10</v>
-      </c>
-      <c r="E19" s="1">
-        <v>5</v>
-      </c>
-      <c r="F19" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="F20" s="1">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="1">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1">
-        <v>10</v>
-      </c>
-      <c r="E20" s="1">
-        <v>5</v>
-      </c>
-      <c r="F20" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="1">
-        <v>3</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F21" s="1">
-        <v>30</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G21" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>